<commit_message>
Update of databases: DeltaG0f and DeltaH0f
</commit_message>
<xml_diff>
--- a/ecosysem/db/Excels/DeltaG0f.xlsx
+++ b/ecosysem/db/Excels/DeltaG0f.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\EcoSysEM\ecosysem\db\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E320F1D-EC8E-4959-B8F4-796B4FCADFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2AC8F5-248F-4AB9-BDF2-0B9737844A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A62AFDAB-FBC8-40CE-9878-3FD750A8957F}"/>
+    <workbookView xWindow="-23148" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{A62AFDAB-FBC8-40CE-9878-3FD750A8957F}"/>
   </bookViews>
   <sheets>
     <sheet name="DeltaG" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="77">
   <si>
     <t>IUPAC</t>
   </si>
@@ -285,6 +285,15 @@
   </si>
   <si>
     <t>Sulfur dioxide</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Sulfur (rhombic)</t>
   </si>
 </sst>
 </file>
@@ -688,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC731D4-E3C1-4B64-BF1D-C3C9432561A9}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1416,6 +1425,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>